<commit_message>
Se solucionan errores con el boton de inicio
</commit_message>
<xml_diff>
--- a/Test/Data/tareas.xlsx
+++ b/Test/Data/tareas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjpre\RiderProjects\265403_243045_174039\Test\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flopa\RiderProjects\265403_243045_174039\Test\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EAD2A4-4CFD-4318-A9A5-73F8DBA2B81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413EBDCF-72DC-4F1A-8A39-3D6763D40097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{2B55C6BB-B0FB-40BC-AA64-7EBD9D63A054}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2B55C6BB-B0FB-40BC-AA64-7EBD9D63A054}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Título</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Contactar al cliente para actualizar el estado del proyecto.</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Pagar proveedores</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>Terminar el obligatorio 2 de DA.</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>Comprar mesa ping pong</t>
@@ -151,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -470,12 +464,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -492,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -508,68 +502,68 @@
       <c r="C2" s="1">
         <v>45910</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>45919</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
+      <c r="F3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>45981</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
+      <c r="F4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>46015</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5">
         <v>2</v>

</xml_diff>